<commit_message>
fix and add config
</commit_message>
<xml_diff>
--- a/Data/Example_Excel_Template.xlsx
+++ b/Data/Example_Excel_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff003247ba18f7a0/Bureau/BeCode/LGG-Thomas4-LauraK/projects/openspace_organizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atome\Desktop\becode\SynologyDrive\projet\challenge-openspace-classifier\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_966C8C74A3E015F5E69569B7D26760A574E46D3D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E5E1E79-D1C8-4F7F-8A04-4CC56882C787}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845F220D-C85C-4DE9-86EB-483D7053946D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2205" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Colleagues</t>
   </si>
@@ -371,19 +371,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -417,118 +417,128 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>